<commit_message>
minor bug fixes and adjusted example models to new GAMS interface - added hard gams interrupt in case processx kill_tree fails
</commit_message>
<xml_diff>
--- a/model/pickstock/pickstock.xlsx
+++ b/model/pickstock/pickstock.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="stockData" sheetId="1" r:id="rId1"/>
+    <sheet name="price" sheetId="1" r:id="rId1"/>
     <sheet name="scalars" sheetId="2" r:id="rId2"/>
     <sheet name="partOfPortfolio" sheetId="3" r:id="rId3"/>
     <sheet name="dowVSindex" sheetId="4" r:id="rId4"/>
@@ -27,7 +27,7 @@
     <t>stockSymbol</t>
   </si>
   <si>
-    <t>price</t>
+    <t>Price</t>
   </si>
   <si>
     <t>2016-01-04</t>
@@ -897,7 +897,7 @@
     <t>number of days for training</t>
   </si>
   <si>
-    <t>weight</t>
+    <t>what part of the portfolio</t>
   </si>
   <si>
     <t>dow jones</t>
@@ -84495,9 +84495,6 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>